<commit_message>
update the sample project
</commit_message>
<xml_diff>
--- a/sample lightweight domain/resources/domains/countries.xlsx
+++ b/sample lightweight domain/resources/domains/countries.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FREDERICMercier\Desktop\VALUE PROVIDER\1- mine\workspace\Value Provider BOM customization\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IBM\GitHub\dc-lightweight-domain\sample lightweight domain\resources\domains\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7770F3BA-F9ED-4CEF-8506-888B494A0102}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45C7560-C407-42C0-B3AF-E5ED0ED750B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6900" yWindow="3975" windowWidth="21600" windowHeight="11430" xr2:uid="{191EE4D9-30B1-4391-94EB-FEF0069EDE9A}"/>
+    <workbookView xWindow="15" yWindow="5010" windowWidth="28740" windowHeight="10620" xr2:uid="{191EE4D9-30B1-4391-94EB-FEF0069EDE9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="198">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -576,15 +576,6 @@
     <t>Benin</t>
   </si>
   <si>
-    <t>return "ELSA";</t>
-  </si>
-  <si>
-    <t>return "UKIN";</t>
-  </si>
-  <si>
-    <t>return "TURM";</t>
-  </si>
-  <si>
     <t>United Kingdom</t>
   </si>
   <si>
@@ -597,9 +588,6 @@
     <t>South Korea</t>
   </si>
   <si>
-    <t>return "SOUK";</t>
-  </si>
-  <si>
     <t>Netherlands</t>
   </si>
   <si>
@@ -616,6 +604,30 @@
   </si>
   <si>
     <t>Burkina Faso</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>UAE</t>
+  </si>
+  <si>
+    <t>TURM</t>
+  </si>
+  <si>
+    <t>SLA</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>NIGA</t>
+  </si>
+  <si>
+    <t>AUS</t>
+  </si>
+  <si>
+    <t>MALW</t>
   </si>
 </sst>
 </file>
@@ -969,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{746568ED-BE32-48AD-BB23-CCB4654E692A}">
   <dimension ref="A1:C188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,8 +1007,8 @@
         <v>Afghanistan</v>
       </c>
       <c r="B2" t="str">
-        <f>CONCATENATE("return """, UPPER(LEFT(A2,4)), """;")</f>
-        <v>return "AFGH";</v>
+        <f t="shared" ref="B2:B65" si="0">UPPER(LEFT(A2,4))</f>
+        <v>AFGH</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -1004,12 +1016,12 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
-        <f t="shared" ref="A3:A64" si="0">SUBSTITUTE(C3, " ", "_")</f>
+        <f t="shared" ref="A3:A64" si="1">SUBSTITUTE(C3, " ", "_")</f>
         <v>Albania</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B62" si="1">CONCATENATE("return """, UPPER(LEFT(A3,4)), """;")</f>
-        <v>return "ALBA";</v>
+        <f t="shared" si="0"/>
+        <v>ALBA</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -1017,12 +1029,12 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Algeria</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" si="1"/>
-        <v>return "ALGE";</v>
+        <f t="shared" si="0"/>
+        <v>ALGE</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -1030,12 +1042,12 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Andorra</v>
       </c>
       <c r="B5" t="str">
-        <f t="shared" si="1"/>
-        <v>return "ANDO";</v>
+        <f t="shared" si="0"/>
+        <v>ANDO</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -1043,12 +1055,12 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Angola</v>
       </c>
       <c r="B6" t="str">
-        <f t="shared" si="1"/>
-        <v>return "ANGO";</v>
+        <f t="shared" si="0"/>
+        <v>ANGO</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1056,12 +1068,12 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Antigua_and_Barbuda</v>
       </c>
       <c r="B7" t="str">
-        <f t="shared" si="1"/>
-        <v>return "ANTI";</v>
+        <f t="shared" si="0"/>
+        <v>ANTI</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -1069,12 +1081,12 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Argentina</v>
       </c>
       <c r="B8" t="str">
-        <f t="shared" si="1"/>
-        <v>return "ARGE";</v>
+        <f t="shared" si="0"/>
+        <v>ARGE</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -1082,12 +1094,12 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Armenia</v>
       </c>
       <c r="B9" t="str">
-        <f t="shared" si="1"/>
-        <v>return "ARME";</v>
+        <f t="shared" si="0"/>
+        <v>ARME</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -1095,12 +1107,11 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Australia</v>
       </c>
-      <c r="B10" t="str">
-        <f t="shared" si="1"/>
-        <v>return "AUST";</v>
+      <c r="B10" t="s">
+        <v>196</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -1108,12 +1119,12 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Austria</v>
       </c>
       <c r="B11" t="str">
-        <f t="shared" si="1"/>
-        <v>return "AUST";</v>
+        <f t="shared" si="0"/>
+        <v>AUST</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -1121,12 +1132,12 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Azerbaijan</v>
       </c>
       <c r="B12" t="str">
-        <f t="shared" si="1"/>
-        <v>return "AZER";</v>
+        <f t="shared" si="0"/>
+        <v>AZER</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -1134,12 +1145,12 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Bahamas</v>
       </c>
       <c r="B13" t="str">
-        <f t="shared" si="1"/>
-        <v>return "BAHA";</v>
+        <f t="shared" si="0"/>
+        <v>BAHA</v>
       </c>
       <c r="C13" t="s">
         <v>178</v>
@@ -1147,12 +1158,12 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Bahrain</v>
       </c>
       <c r="B14" t="str">
-        <f t="shared" si="1"/>
-        <v>return "BAHR";</v>
+        <f t="shared" si="0"/>
+        <v>BAHR</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -1160,12 +1171,12 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Bangladesh</v>
       </c>
       <c r="B15" t="str">
-        <f t="shared" si="1"/>
-        <v>return "BANG";</v>
+        <f t="shared" si="0"/>
+        <v>BANG</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
@@ -1173,12 +1184,12 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Barbados</v>
       </c>
       <c r="B16" t="str">
-        <f t="shared" si="1"/>
-        <v>return "BARB";</v>
+        <f t="shared" si="0"/>
+        <v>BARB</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
@@ -1186,12 +1197,12 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Belarus</v>
       </c>
       <c r="B17" t="str">
-        <f t="shared" si="1"/>
-        <v>return "BELA";</v>
+        <f t="shared" si="0"/>
+        <v>BELA</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
@@ -1199,12 +1210,12 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Belgium</v>
       </c>
       <c r="B18" t="str">
-        <f t="shared" si="1"/>
-        <v>return "BELG";</v>
+        <f t="shared" si="0"/>
+        <v>BELG</v>
       </c>
       <c r="C18" t="s">
         <v>15</v>
@@ -1212,12 +1223,12 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Benin</v>
       </c>
       <c r="B19" t="str">
-        <f t="shared" si="1"/>
-        <v>return "BENI";</v>
+        <f t="shared" si="0"/>
+        <v>BENI</v>
       </c>
       <c r="C19" t="s">
         <v>179</v>
@@ -1225,12 +1236,12 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Bolivia</v>
       </c>
       <c r="B20" t="str">
-        <f t="shared" si="1"/>
-        <v>return "BOLI";</v>
+        <f t="shared" si="0"/>
+        <v>BOLI</v>
       </c>
       <c r="C20" t="s">
         <v>16</v>
@@ -1238,12 +1249,12 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Bosnia_and_Herzegovina</v>
       </c>
       <c r="B21" t="str">
-        <f t="shared" si="1"/>
-        <v>return "BOSN";</v>
+        <f t="shared" si="0"/>
+        <v>BOSN</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
@@ -1251,12 +1262,12 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Botswana</v>
       </c>
       <c r="B22" t="str">
-        <f t="shared" si="1"/>
-        <v>return "BOTS";</v>
+        <f t="shared" si="0"/>
+        <v>BOTS</v>
       </c>
       <c r="C22" t="s">
         <v>18</v>
@@ -1264,12 +1275,12 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Brazil</v>
       </c>
       <c r="B23" t="str">
-        <f t="shared" si="1"/>
-        <v>return "BRAZ";</v>
+        <f t="shared" si="0"/>
+        <v>BRAZ</v>
       </c>
       <c r="C23" t="s">
         <v>19</v>
@@ -1277,12 +1288,12 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Brunei</v>
       </c>
       <c r="B24" t="str">
-        <f t="shared" si="1"/>
-        <v>return "BRUN";</v>
+        <f t="shared" si="0"/>
+        <v>BRUN</v>
       </c>
       <c r="C24" t="s">
         <v>20</v>
@@ -1290,12 +1301,12 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Bulgaria</v>
       </c>
       <c r="B25" t="str">
-        <f t="shared" si="1"/>
-        <v>return "BULG";</v>
+        <f t="shared" si="0"/>
+        <v>BULG</v>
       </c>
       <c r="C25" t="s">
         <v>21</v>
@@ -1303,25 +1314,25 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Burkina_Faso</v>
       </c>
       <c r="B26" t="str">
-        <f t="shared" si="1"/>
-        <v>return "BURK";</v>
+        <f t="shared" si="0"/>
+        <v>BURK</v>
       </c>
       <c r="C26" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Burundi</v>
       </c>
       <c r="B27" t="str">
-        <f t="shared" si="1"/>
-        <v>return "BURU";</v>
+        <f t="shared" si="0"/>
+        <v>BURU</v>
       </c>
       <c r="C27" t="s">
         <v>22</v>
@@ -1329,12 +1340,12 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Cabo_Verde</v>
       </c>
       <c r="B28" t="str">
-        <f t="shared" si="1"/>
-        <v>return "CABO";</v>
+        <f t="shared" si="0"/>
+        <v>CABO</v>
       </c>
       <c r="C28" t="s">
         <v>23</v>
@@ -1342,12 +1353,12 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Cambodia</v>
       </c>
       <c r="B29" t="str">
-        <f t="shared" si="1"/>
-        <v>return "CAMB";</v>
+        <f t="shared" si="0"/>
+        <v>CAMB</v>
       </c>
       <c r="C29" t="s">
         <v>24</v>
@@ -1355,12 +1366,12 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Cameroon</v>
       </c>
       <c r="B30" t="str">
-        <f t="shared" si="1"/>
-        <v>return "CAME";</v>
+        <f t="shared" si="0"/>
+        <v>CAME</v>
       </c>
       <c r="C30" t="s">
         <v>25</v>
@@ -1368,12 +1379,12 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Canada</v>
       </c>
       <c r="B31" t="str">
-        <f t="shared" si="1"/>
-        <v>return "CANA";</v>
+        <f t="shared" si="0"/>
+        <v>CANA</v>
       </c>
       <c r="C31" t="s">
         <v>26</v>
@@ -1381,25 +1392,25 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Cayman_Islands</v>
       </c>
       <c r="B32" t="str">
-        <f t="shared" si="1"/>
-        <v>return "CAYM";</v>
+        <f t="shared" si="0"/>
+        <v>CAYM</v>
       </c>
       <c r="C32" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Central_African_Republic</v>
       </c>
       <c r="B33" t="str">
-        <f t="shared" si="1"/>
-        <v>return "CENT";</v>
+        <f t="shared" si="0"/>
+        <v>CENT</v>
       </c>
       <c r="C33" t="s">
         <v>27</v>
@@ -1407,12 +1418,12 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Chad</v>
       </c>
       <c r="B34" t="str">
-        <f t="shared" si="1"/>
-        <v>return "CHAD";</v>
+        <f t="shared" si="0"/>
+        <v>CHAD</v>
       </c>
       <c r="C34" t="s">
         <v>28</v>
@@ -1420,12 +1431,12 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Chile</v>
       </c>
       <c r="B35" t="str">
-        <f t="shared" si="1"/>
-        <v>return "CHIL";</v>
+        <f t="shared" si="0"/>
+        <v>CHIL</v>
       </c>
       <c r="C35" t="s">
         <v>29</v>
@@ -1433,12 +1444,12 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>China</v>
       </c>
       <c r="B36" t="str">
-        <f t="shared" si="1"/>
-        <v>return "CHIN";</v>
+        <f t="shared" si="0"/>
+        <v>CHIN</v>
       </c>
       <c r="C36" t="s">
         <v>30</v>
@@ -1446,12 +1457,12 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Colombia</v>
       </c>
       <c r="B37" t="str">
-        <f t="shared" si="1"/>
-        <v>return "COLO";</v>
+        <f t="shared" si="0"/>
+        <v>COLO</v>
       </c>
       <c r="C37" t="s">
         <v>31</v>
@@ -1459,12 +1470,12 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Comoros</v>
       </c>
       <c r="B38" t="str">
-        <f t="shared" si="1"/>
-        <v>return "COMO";</v>
+        <f t="shared" si="0"/>
+        <v>COMO</v>
       </c>
       <c r="C38" t="s">
         <v>32</v>
@@ -1472,25 +1483,25 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Congo_Free_State</v>
       </c>
       <c r="B39" t="str">
-        <f t="shared" si="1"/>
-        <v>return "CONG";</v>
+        <f t="shared" si="0"/>
+        <v>CONG</v>
       </c>
       <c r="C39" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Costa_Rica</v>
       </c>
       <c r="B40" t="str">
-        <f t="shared" si="1"/>
-        <v>return "COST";</v>
+        <f t="shared" si="0"/>
+        <v>COST</v>
       </c>
       <c r="C40" t="s">
         <v>33</v>
@@ -1498,12 +1509,12 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Croatia</v>
       </c>
       <c r="B41" t="str">
-        <f t="shared" si="1"/>
-        <v>return "CROA";</v>
+        <f t="shared" si="0"/>
+        <v>CROA</v>
       </c>
       <c r="C41" t="s">
         <v>34</v>
@@ -1511,12 +1522,12 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Cuba</v>
       </c>
       <c r="B42" t="str">
-        <f t="shared" si="1"/>
-        <v>return "CUBA";</v>
+        <f t="shared" si="0"/>
+        <v>CUBA</v>
       </c>
       <c r="C42" t="s">
         <v>35</v>
@@ -1524,12 +1535,12 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Cyprus</v>
       </c>
       <c r="B43" t="str">
-        <f t="shared" si="1"/>
-        <v>return "CYPR";</v>
+        <f t="shared" si="0"/>
+        <v>CYPR</v>
       </c>
       <c r="C43" t="s">
         <v>36</v>
@@ -1537,12 +1548,12 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Czechoslovakia</v>
       </c>
       <c r="B44" t="str">
-        <f t="shared" si="1"/>
-        <v>return "CZEC";</v>
+        <f t="shared" si="0"/>
+        <v>CZEC</v>
       </c>
       <c r="C44" t="s">
         <v>37</v>
@@ -1550,12 +1561,12 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Democratic_Republic_of_the_Congo</v>
       </c>
       <c r="B45" t="str">
-        <f t="shared" si="1"/>
-        <v>return "DEMO";</v>
+        <f t="shared" si="0"/>
+        <v>DEMO</v>
       </c>
       <c r="C45" t="s">
         <v>38</v>
@@ -1563,12 +1574,12 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Denmark</v>
       </c>
       <c r="B46" t="str">
-        <f t="shared" si="1"/>
-        <v>return "DENM";</v>
+        <f t="shared" si="0"/>
+        <v>DENM</v>
       </c>
       <c r="C46" t="s">
         <v>39</v>
@@ -1576,12 +1587,12 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Djibouti</v>
       </c>
       <c r="B47" t="str">
-        <f t="shared" si="1"/>
-        <v>return "DJIB";</v>
+        <f t="shared" si="0"/>
+        <v>DJIB</v>
       </c>
       <c r="C47" t="s">
         <v>40</v>
@@ -1589,12 +1600,12 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Dominican_Republic</v>
       </c>
       <c r="B48" t="str">
-        <f t="shared" si="1"/>
-        <v>return "DOMI";</v>
+        <f t="shared" si="0"/>
+        <v>DOMI</v>
       </c>
       <c r="C48" t="s">
         <v>41</v>
@@ -1602,12 +1613,12 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Ecuador</v>
       </c>
       <c r="B49" t="str">
-        <f t="shared" si="1"/>
-        <v>return "ECUA";</v>
+        <f t="shared" si="0"/>
+        <v>ECUA</v>
       </c>
       <c r="C49" t="s">
         <v>42</v>
@@ -1615,12 +1626,12 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Egypt</v>
       </c>
       <c r="B50" t="str">
-        <f t="shared" si="1"/>
-        <v>return "EGYP";</v>
+        <f t="shared" si="0"/>
+        <v>EGYP</v>
       </c>
       <c r="C50" t="s">
         <v>43</v>
@@ -1628,11 +1639,12 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>El_Salvador</v>
       </c>
-      <c r="B51" t="s">
-        <v>180</v>
+      <c r="B51" t="str">
+        <f t="shared" si="0"/>
+        <v>EL_S</v>
       </c>
       <c r="C51" t="s">
         <v>44</v>
@@ -1640,12 +1652,12 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Equatorial_Guinea</v>
       </c>
       <c r="B52" t="str">
-        <f t="shared" si="1"/>
-        <v>return "EQUA";</v>
+        <f t="shared" si="0"/>
+        <v>EQUA</v>
       </c>
       <c r="C52" t="s">
         <v>45</v>
@@ -1653,12 +1665,12 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Eritrea</v>
       </c>
       <c r="B53" t="str">
-        <f t="shared" si="1"/>
-        <v>return "ERIT";</v>
+        <f t="shared" si="0"/>
+        <v>ERIT</v>
       </c>
       <c r="C53" t="s">
         <v>46</v>
@@ -1666,12 +1678,12 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Estonia</v>
       </c>
       <c r="B54" t="str">
-        <f t="shared" si="1"/>
-        <v>return "ESTO";</v>
+        <f t="shared" si="0"/>
+        <v>ESTO</v>
       </c>
       <c r="C54" t="s">
         <v>47</v>
@@ -1679,12 +1691,12 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Eswatini</v>
       </c>
       <c r="B55" t="str">
-        <f t="shared" si="1"/>
-        <v>return "ESWA";</v>
+        <f t="shared" si="0"/>
+        <v>ESWA</v>
       </c>
       <c r="C55" t="s">
         <v>48</v>
@@ -1692,12 +1704,12 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Ethiopia</v>
       </c>
       <c r="B56" t="str">
-        <f t="shared" si="1"/>
-        <v>return "ETHI";</v>
+        <f t="shared" si="0"/>
+        <v>ETHI</v>
       </c>
       <c r="C56" t="s">
         <v>49</v>
@@ -1705,12 +1717,12 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Fiji</v>
       </c>
       <c r="B57" t="str">
-        <f t="shared" si="1"/>
-        <v>return "FIJI";</v>
+        <f t="shared" si="0"/>
+        <v>FIJI</v>
       </c>
       <c r="C57" t="s">
         <v>50</v>
@@ -1718,12 +1730,12 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Finland</v>
       </c>
       <c r="B58" t="str">
-        <f t="shared" si="1"/>
-        <v>return "FINL";</v>
+        <f t="shared" si="0"/>
+        <v>FINL</v>
       </c>
       <c r="C58" t="s">
         <v>51</v>
@@ -1731,12 +1743,12 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>France</v>
       </c>
       <c r="B59" t="str">
-        <f t="shared" si="1"/>
-        <v>return "FRAN";</v>
+        <f t="shared" si="0"/>
+        <v>FRAN</v>
       </c>
       <c r="C59" t="s">
         <v>52</v>
@@ -1744,12 +1756,12 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Gabon</v>
       </c>
       <c r="B60" t="str">
-        <f t="shared" si="1"/>
-        <v>return "GABO";</v>
+        <f t="shared" si="0"/>
+        <v>GABO</v>
       </c>
       <c r="C60" t="s">
         <v>53</v>
@@ -1757,25 +1769,25 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Gambia</v>
       </c>
       <c r="B61" t="str">
-        <f t="shared" si="1"/>
-        <v>return "GAMB";</v>
+        <f t="shared" si="0"/>
+        <v>GAMB</v>
       </c>
       <c r="C61" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Georgia</v>
       </c>
       <c r="B62" t="str">
-        <f t="shared" si="1"/>
-        <v>return "GEOR";</v>
+        <f t="shared" si="0"/>
+        <v>GEOR</v>
       </c>
       <c r="C62" t="s">
         <v>54</v>
@@ -1783,12 +1795,12 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Germany</v>
       </c>
       <c r="B63" t="str">
-        <f t="shared" ref="B63:B125" si="2">CONCATENATE("return """, UPPER(LEFT(A63,4)), """;")</f>
-        <v>return "GERM";</v>
+        <f t="shared" si="0"/>
+        <v>GERM</v>
       </c>
       <c r="C63" t="s">
         <v>55</v>
@@ -1796,12 +1808,12 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Ghana</v>
       </c>
       <c r="B64" t="str">
-        <f t="shared" si="2"/>
-        <v>return "GHAN";</v>
+        <f t="shared" si="0"/>
+        <v>GHAN</v>
       </c>
       <c r="C64" t="s">
         <v>56</v>
@@ -1809,12 +1821,12 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
-        <f t="shared" ref="A65:A129" si="3">SUBSTITUTE(C65, " ", "_")</f>
+        <f t="shared" ref="A65:A129" si="2">SUBSTITUTE(C65, " ", "_")</f>
         <v>Greece</v>
       </c>
       <c r="B65" t="str">
-        <f t="shared" si="2"/>
-        <v>return "GREE";</v>
+        <f t="shared" si="0"/>
+        <v>GREE</v>
       </c>
       <c r="C65" t="s">
         <v>57</v>
@@ -1822,12 +1834,12 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Grenada</v>
       </c>
       <c r="B66" t="str">
-        <f t="shared" si="2"/>
-        <v>return "GREN";</v>
+        <f t="shared" ref="B66:B129" si="3">UPPER(LEFT(A66,4))</f>
+        <v>GREN</v>
       </c>
       <c r="C66" t="s">
         <v>58</v>
@@ -1835,12 +1847,12 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Guatemala</v>
       </c>
       <c r="B67" t="str">
-        <f t="shared" si="2"/>
-        <v>return "GUAT";</v>
+        <f t="shared" si="3"/>
+        <v>GUAT</v>
       </c>
       <c r="C67" t="s">
         <v>59</v>
@@ -1848,12 +1860,12 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Guinea</v>
       </c>
       <c r="B68" t="str">
-        <f t="shared" si="2"/>
-        <v>return "GUIN";</v>
+        <f t="shared" si="3"/>
+        <v>GUIN</v>
       </c>
       <c r="C68" t="s">
         <v>60</v>
@@ -1861,12 +1873,12 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Guyana</v>
       </c>
       <c r="B69" t="str">
-        <f t="shared" si="2"/>
-        <v>return "GUYA";</v>
+        <f t="shared" si="3"/>
+        <v>GUYA</v>
       </c>
       <c r="C69" t="s">
         <v>61</v>
@@ -1874,12 +1886,12 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Haiti</v>
       </c>
       <c r="B70" t="str">
-        <f t="shared" si="2"/>
-        <v>return "HAIT";</v>
+        <f t="shared" si="3"/>
+        <v>HAIT</v>
       </c>
       <c r="C70" t="s">
         <v>62</v>
@@ -1887,12 +1899,12 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Holy_See</v>
       </c>
       <c r="B71" t="str">
-        <f t="shared" si="2"/>
-        <v>return "HOLY";</v>
+        <f t="shared" si="3"/>
+        <v>HOLY</v>
       </c>
       <c r="C71" t="s">
         <v>63</v>
@@ -1900,12 +1912,12 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Honduras</v>
       </c>
       <c r="B72" t="str">
-        <f t="shared" si="2"/>
-        <v>return "HOND";</v>
+        <f t="shared" si="3"/>
+        <v>HOND</v>
       </c>
       <c r="C72" t="s">
         <v>64</v>
@@ -1913,12 +1925,12 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Hungary</v>
       </c>
       <c r="B73" t="str">
-        <f t="shared" si="2"/>
-        <v>return "HUNG";</v>
+        <f t="shared" si="3"/>
+        <v>HUNG</v>
       </c>
       <c r="C73" t="s">
         <v>65</v>
@@ -1926,12 +1938,12 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Iceland</v>
       </c>
       <c r="B74" t="str">
-        <f t="shared" si="2"/>
-        <v>return "ICEL";</v>
+        <f t="shared" si="3"/>
+        <v>ICEL</v>
       </c>
       <c r="C74" t="s">
         <v>66</v>
@@ -1939,12 +1951,12 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>India</v>
       </c>
       <c r="B75" t="str">
-        <f t="shared" si="2"/>
-        <v>return "INDI";</v>
+        <f t="shared" si="3"/>
+        <v>INDI</v>
       </c>
       <c r="C75" t="s">
         <v>67</v>
@@ -1952,12 +1964,12 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Indonesia</v>
       </c>
       <c r="B76" t="str">
-        <f t="shared" si="2"/>
-        <v>return "INDO";</v>
+        <f t="shared" si="3"/>
+        <v>INDO</v>
       </c>
       <c r="C76" t="s">
         <v>68</v>
@@ -1965,12 +1977,12 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Iran</v>
       </c>
       <c r="B77" t="str">
-        <f t="shared" si="2"/>
-        <v>return "IRAN";</v>
+        <f t="shared" si="3"/>
+        <v>IRAN</v>
       </c>
       <c r="C77" t="s">
         <v>69</v>
@@ -1978,12 +1990,12 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Iraq</v>
       </c>
       <c r="B78" t="str">
-        <f t="shared" si="2"/>
-        <v>return "IRAQ";</v>
+        <f t="shared" si="3"/>
+        <v>IRAQ</v>
       </c>
       <c r="C78" t="s">
         <v>70</v>
@@ -1991,12 +2003,12 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Ireland</v>
       </c>
       <c r="B79" t="str">
-        <f t="shared" si="2"/>
-        <v>return "IREL";</v>
+        <f t="shared" si="3"/>
+        <v>IREL</v>
       </c>
       <c r="C79" t="s">
         <v>71</v>
@@ -2004,12 +2016,12 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Israel</v>
       </c>
       <c r="B80" t="str">
-        <f t="shared" si="2"/>
-        <v>return "ISRA";</v>
+        <f t="shared" si="3"/>
+        <v>ISRA</v>
       </c>
       <c r="C80" t="s">
         <v>72</v>
@@ -2017,12 +2029,12 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Italy</v>
       </c>
       <c r="B81" t="str">
-        <f t="shared" si="2"/>
-        <v>return "ITAL";</v>
+        <f t="shared" si="3"/>
+        <v>ITAL</v>
       </c>
       <c r="C81" t="s">
         <v>73</v>
@@ -2034,21 +2046,21 @@
         <v>Ivory_Coast</v>
       </c>
       <c r="B82" t="str">
-        <f>CONCATENATE("return """, UPPER(LEFT(A82,4)), """;")</f>
-        <v>return "IVOR";</v>
+        <f t="shared" si="3"/>
+        <v>IVOR</v>
       </c>
       <c r="C82" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Jamaica</v>
       </c>
       <c r="B83" t="str">
-        <f t="shared" si="2"/>
-        <v>return "JAMA";</v>
+        <f t="shared" si="3"/>
+        <v>JAMA</v>
       </c>
       <c r="C83" t="s">
         <v>74</v>
@@ -2056,12 +2068,12 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Japan</v>
       </c>
       <c r="B84" t="str">
-        <f t="shared" si="2"/>
-        <v>return "JAPA";</v>
+        <f t="shared" si="3"/>
+        <v>JAPA</v>
       </c>
       <c r="C84" t="s">
         <v>75</v>
@@ -2069,12 +2081,12 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Jordan</v>
       </c>
       <c r="B85" t="str">
-        <f t="shared" si="2"/>
-        <v>return "JORD";</v>
+        <f t="shared" si="3"/>
+        <v>JORD</v>
       </c>
       <c r="C85" t="s">
         <v>76</v>
@@ -2082,12 +2094,12 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Kazakhstan</v>
       </c>
       <c r="B86" t="str">
-        <f t="shared" si="2"/>
-        <v>return "KAZA";</v>
+        <f t="shared" si="3"/>
+        <v>KAZA</v>
       </c>
       <c r="C86" t="s">
         <v>77</v>
@@ -2095,12 +2107,12 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Kenya</v>
       </c>
       <c r="B87" t="str">
-        <f t="shared" si="2"/>
-        <v>return "KENY";</v>
+        <f t="shared" si="3"/>
+        <v>KENY</v>
       </c>
       <c r="C87" t="s">
         <v>78</v>
@@ -2108,12 +2120,12 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Kiribati</v>
       </c>
       <c r="B88" t="str">
-        <f t="shared" si="2"/>
-        <v>return "KIRI";</v>
+        <f t="shared" si="3"/>
+        <v>KIRI</v>
       </c>
       <c r="C88" t="s">
         <v>79</v>
@@ -2121,12 +2133,12 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Korea</v>
       </c>
       <c r="B89" t="str">
-        <f t="shared" si="2"/>
-        <v>return "KORE";</v>
+        <f t="shared" si="3"/>
+        <v>KORE</v>
       </c>
       <c r="C89" t="s">
         <v>80</v>
@@ -2134,12 +2146,12 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Kosovo</v>
       </c>
       <c r="B90" t="str">
-        <f t="shared" si="2"/>
-        <v>return "KOSO";</v>
+        <f t="shared" si="3"/>
+        <v>KOSO</v>
       </c>
       <c r="C90" t="s">
         <v>81</v>
@@ -2147,12 +2159,12 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Kuwait</v>
       </c>
       <c r="B91" t="str">
-        <f t="shared" si="2"/>
-        <v>return "KUWA";</v>
+        <f t="shared" si="3"/>
+        <v>KUWA</v>
       </c>
       <c r="C91" t="s">
         <v>82</v>
@@ -2160,12 +2172,12 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Kyrgyzstan</v>
       </c>
       <c r="B92" t="str">
-        <f t="shared" si="2"/>
-        <v>return "KYRG";</v>
+        <f t="shared" si="3"/>
+        <v>KYRG</v>
       </c>
       <c r="C92" t="s">
         <v>83</v>
@@ -2173,12 +2185,12 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Laos</v>
       </c>
       <c r="B93" t="str">
-        <f t="shared" si="2"/>
-        <v>return "LAOS";</v>
+        <f t="shared" si="3"/>
+        <v>LAOS</v>
       </c>
       <c r="C93" t="s">
         <v>84</v>
@@ -2186,12 +2198,12 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Latvia</v>
       </c>
       <c r="B94" t="str">
-        <f t="shared" si="2"/>
-        <v>return "LATV";</v>
+        <f t="shared" si="3"/>
+        <v>LATV</v>
       </c>
       <c r="C94" t="s">
         <v>85</v>
@@ -2199,12 +2211,12 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Lebanon</v>
       </c>
       <c r="B95" t="str">
-        <f t="shared" si="2"/>
-        <v>return "LEBA";</v>
+        <f t="shared" si="3"/>
+        <v>LEBA</v>
       </c>
       <c r="C95" t="s">
         <v>86</v>
@@ -2212,12 +2224,12 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Lesotho</v>
       </c>
       <c r="B96" t="str">
-        <f t="shared" si="2"/>
-        <v>return "LESO";</v>
+        <f t="shared" si="3"/>
+        <v>LESO</v>
       </c>
       <c r="C96" t="s">
         <v>87</v>
@@ -2225,12 +2237,12 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Liberia</v>
       </c>
       <c r="B97" t="str">
-        <f t="shared" si="2"/>
-        <v>return "LIBE";</v>
+        <f t="shared" si="3"/>
+        <v>LIBE</v>
       </c>
       <c r="C97" t="s">
         <v>88</v>
@@ -2238,12 +2250,12 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Libya</v>
       </c>
       <c r="B98" t="str">
-        <f t="shared" si="2"/>
-        <v>return "LIBY";</v>
+        <f t="shared" si="3"/>
+        <v>LIBY</v>
       </c>
       <c r="C98" t="s">
         <v>89</v>
@@ -2251,12 +2263,12 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Liechtenstein</v>
       </c>
       <c r="B99" t="str">
-        <f t="shared" si="2"/>
-        <v>return "LIEC";</v>
+        <f t="shared" si="3"/>
+        <v>LIEC</v>
       </c>
       <c r="C99" t="s">
         <v>90</v>
@@ -2264,12 +2276,12 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Lithuania</v>
       </c>
       <c r="B100" t="str">
-        <f t="shared" si="2"/>
-        <v>return "LITH";</v>
+        <f t="shared" si="3"/>
+        <v>LITH</v>
       </c>
       <c r="C100" t="s">
         <v>91</v>
@@ -2277,12 +2289,12 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Luxembourg</v>
       </c>
       <c r="B101" t="str">
-        <f t="shared" si="2"/>
-        <v>return "LUXE";</v>
+        <f t="shared" si="3"/>
+        <v>LUXE</v>
       </c>
       <c r="C101" t="s">
         <v>92</v>
@@ -2290,12 +2302,12 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Madagascar</v>
       </c>
       <c r="B102" t="str">
-        <f t="shared" si="2"/>
-        <v>return "MADA";</v>
+        <f t="shared" si="3"/>
+        <v>MADA</v>
       </c>
       <c r="C102" t="s">
         <v>93</v>
@@ -2303,12 +2315,11 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Malawi</v>
       </c>
-      <c r="B103" t="str">
-        <f t="shared" si="2"/>
-        <v>return "MALA";</v>
+      <c r="B103" t="s">
+        <v>197</v>
       </c>
       <c r="C103" t="s">
         <v>94</v>
@@ -2316,12 +2327,12 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Malaysia</v>
       </c>
       <c r="B104" t="str">
-        <f t="shared" si="2"/>
-        <v>return "MALA";</v>
+        <f t="shared" si="3"/>
+        <v>MALA</v>
       </c>
       <c r="C104" t="s">
         <v>95</v>
@@ -2329,12 +2340,12 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Maldives</v>
       </c>
       <c r="B105" t="str">
-        <f t="shared" si="2"/>
-        <v>return "MALD";</v>
+        <f t="shared" si="3"/>
+        <v>MALD</v>
       </c>
       <c r="C105" t="s">
         <v>96</v>
@@ -2342,12 +2353,12 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Mali</v>
       </c>
       <c r="B106" t="str">
-        <f t="shared" si="2"/>
-        <v>return "MALI";</v>
+        <f t="shared" si="3"/>
+        <v>MALI</v>
       </c>
       <c r="C106" t="s">
         <v>97</v>
@@ -2355,12 +2366,12 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Malta</v>
       </c>
       <c r="B107" t="str">
-        <f t="shared" si="2"/>
-        <v>return "MALT";</v>
+        <f t="shared" si="3"/>
+        <v>MALT</v>
       </c>
       <c r="C107" t="s">
         <v>98</v>
@@ -2368,12 +2379,12 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Marshall_Islands</v>
       </c>
       <c r="B108" t="str">
-        <f t="shared" si="2"/>
-        <v>return "MARS";</v>
+        <f t="shared" si="3"/>
+        <v>MARS</v>
       </c>
       <c r="C108" t="s">
         <v>99</v>
@@ -2381,12 +2392,12 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Mauritania</v>
       </c>
       <c r="B109" t="str">
-        <f t="shared" si="2"/>
-        <v>return "MAUR";</v>
+        <f t="shared" si="3"/>
+        <v>MAUR</v>
       </c>
       <c r="C109" t="s">
         <v>100</v>
@@ -2394,12 +2405,12 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Mexico</v>
       </c>
       <c r="B110" t="str">
-        <f t="shared" si="2"/>
-        <v>return "MEXI";</v>
+        <f t="shared" si="3"/>
+        <v>MEXI</v>
       </c>
       <c r="C110" t="s">
         <v>101</v>
@@ -2407,12 +2418,12 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Micronesia</v>
       </c>
       <c r="B111" t="str">
-        <f t="shared" si="2"/>
-        <v>return "MICR";</v>
+        <f t="shared" si="3"/>
+        <v>MICR</v>
       </c>
       <c r="C111" t="s">
         <v>102</v>
@@ -2420,12 +2431,12 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Moldova</v>
       </c>
       <c r="B112" t="str">
-        <f t="shared" si="2"/>
-        <v>return "MOLD";</v>
+        <f t="shared" si="3"/>
+        <v>MOLD</v>
       </c>
       <c r="C112" t="s">
         <v>103</v>
@@ -2433,12 +2444,12 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Monaco</v>
       </c>
       <c r="B113" t="str">
-        <f t="shared" si="2"/>
-        <v>return "MONA";</v>
+        <f t="shared" si="3"/>
+        <v>MONA</v>
       </c>
       <c r="C113" t="s">
         <v>104</v>
@@ -2446,12 +2457,12 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Mongolia</v>
       </c>
       <c r="B114" t="str">
-        <f t="shared" si="2"/>
-        <v>return "MONG";</v>
+        <f t="shared" si="3"/>
+        <v>MONG</v>
       </c>
       <c r="C114" t="s">
         <v>105</v>
@@ -2459,12 +2470,12 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Montenegro</v>
       </c>
       <c r="B115" t="str">
-        <f t="shared" si="2"/>
-        <v>return "MONT";</v>
+        <f t="shared" si="3"/>
+        <v>MONT</v>
       </c>
       <c r="C115" t="s">
         <v>106</v>
@@ -2472,12 +2483,12 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Morocco</v>
       </c>
       <c r="B116" t="str">
-        <f t="shared" si="2"/>
-        <v>return "MORO";</v>
+        <f t="shared" si="3"/>
+        <v>MORO</v>
       </c>
       <c r="C116" t="s">
         <v>107</v>
@@ -2485,12 +2496,12 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Mozambique</v>
       </c>
       <c r="B117" t="str">
-        <f t="shared" si="2"/>
-        <v>return "MOZA";</v>
+        <f t="shared" si="3"/>
+        <v>MOZA</v>
       </c>
       <c r="C117" t="s">
         <v>108</v>
@@ -2498,12 +2509,12 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Namibia</v>
       </c>
       <c r="B118" t="str">
-        <f t="shared" si="2"/>
-        <v>return "NAMI";</v>
+        <f t="shared" si="3"/>
+        <v>NAMI</v>
       </c>
       <c r="C118" t="s">
         <v>109</v>
@@ -2511,12 +2522,12 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Nauru</v>
       </c>
       <c r="B119" t="str">
-        <f t="shared" si="2"/>
-        <v>return "NAUR";</v>
+        <f t="shared" si="3"/>
+        <v>NAUR</v>
       </c>
       <c r="C119" t="s">
         <v>110</v>
@@ -2524,12 +2535,12 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Nepal</v>
       </c>
       <c r="B120" t="str">
-        <f t="shared" si="2"/>
-        <v>return "NEPA";</v>
+        <f t="shared" si="3"/>
+        <v>NEPA</v>
       </c>
       <c r="C120" t="s">
         <v>111</v>
@@ -2537,25 +2548,25 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Netherlands</v>
       </c>
       <c r="B121" t="str">
-        <f t="shared" si="2"/>
-        <v>return "NETH";</v>
+        <f t="shared" si="3"/>
+        <v>NETH</v>
       </c>
       <c r="C121" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>New_Zealand</v>
       </c>
       <c r="B122" t="str">
-        <f t="shared" si="2"/>
-        <v>return "NEW_";</v>
+        <f t="shared" si="3"/>
+        <v>NEW_</v>
       </c>
       <c r="C122" t="s">
         <v>112</v>
@@ -2563,12 +2574,12 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Nicaragua</v>
       </c>
       <c r="B123" t="str">
-        <f t="shared" si="2"/>
-        <v>return "NICA";</v>
+        <f t="shared" si="3"/>
+        <v>NICA</v>
       </c>
       <c r="C123" t="s">
         <v>113</v>
@@ -2576,12 +2587,12 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Niger</v>
       </c>
       <c r="B124" t="str">
-        <f t="shared" si="2"/>
-        <v>return "NIGE";</v>
+        <f t="shared" si="3"/>
+        <v>NIGE</v>
       </c>
       <c r="C124" t="s">
         <v>114</v>
@@ -2589,12 +2600,11 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Nigeria</v>
       </c>
-      <c r="B125" t="str">
-        <f t="shared" si="2"/>
-        <v>return "NIGE";</v>
+      <c r="B125" t="s">
+        <v>195</v>
       </c>
       <c r="C125" t="s">
         <v>115</v>
@@ -2602,12 +2612,12 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>North_Macedonia</v>
       </c>
       <c r="B126" t="str">
-        <f t="shared" ref="B126:B186" si="4">CONCATENATE("return """, UPPER(LEFT(A126,4)), """;")</f>
-        <v>return "NORT";</v>
+        <f t="shared" si="3"/>
+        <v>NORT</v>
       </c>
       <c r="C126" t="s">
         <v>116</v>
@@ -2615,12 +2625,12 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Norway</v>
       </c>
       <c r="B127" t="str">
-        <f t="shared" si="4"/>
-        <v>return "NORW";</v>
+        <f t="shared" si="3"/>
+        <v>NORW</v>
       </c>
       <c r="C127" t="s">
         <v>117</v>
@@ -2628,12 +2638,12 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Oman</v>
       </c>
       <c r="B128" t="str">
-        <f t="shared" si="4"/>
-        <v>return "OMAN";</v>
+        <f t="shared" si="3"/>
+        <v>OMAN</v>
       </c>
       <c r="C128" t="s">
         <v>118</v>
@@ -2641,12 +2651,12 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Pakistan</v>
       </c>
       <c r="B129" t="str">
-        <f t="shared" si="4"/>
-        <v>return "PAKI";</v>
+        <f t="shared" si="3"/>
+        <v>PAKI</v>
       </c>
       <c r="C129" t="s">
         <v>119</v>
@@ -2654,12 +2664,12 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="str">
-        <f t="shared" ref="A130:A188" si="5">SUBSTITUTE(C130, " ", "_")</f>
+        <f t="shared" ref="A130:A188" si="4">SUBSTITUTE(C130, " ", "_")</f>
         <v>Palau</v>
       </c>
       <c r="B130" t="str">
-        <f t="shared" si="4"/>
-        <v>return "PALA";</v>
+        <f t="shared" ref="B130:B168" si="5">UPPER(LEFT(A130,4))</f>
+        <v>PALA</v>
       </c>
       <c r="C130" t="s">
         <v>120</v>
@@ -2667,12 +2677,12 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Panama</v>
       </c>
       <c r="B131" t="str">
-        <f t="shared" si="4"/>
-        <v>return "PANA";</v>
+        <f t="shared" si="5"/>
+        <v>PANA</v>
       </c>
       <c r="C131" t="s">
         <v>121</v>
@@ -2680,12 +2690,12 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Papua_New_Guinea</v>
       </c>
       <c r="B132" t="str">
-        <f t="shared" si="4"/>
-        <v>return "PAPU";</v>
+        <f t="shared" si="5"/>
+        <v>PAPU</v>
       </c>
       <c r="C132" t="s">
         <v>122</v>
@@ -2693,12 +2703,12 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Paraguay</v>
       </c>
       <c r="B133" t="str">
-        <f t="shared" si="4"/>
-        <v>return "PARA";</v>
+        <f t="shared" si="5"/>
+        <v>PARA</v>
       </c>
       <c r="C133" t="s">
         <v>123</v>
@@ -2706,12 +2716,12 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Peru</v>
       </c>
       <c r="B134" t="str">
-        <f t="shared" si="4"/>
-        <v>return "PERU";</v>
+        <f t="shared" si="5"/>
+        <v>PERU</v>
       </c>
       <c r="C134" t="s">
         <v>124</v>
@@ -2719,12 +2729,12 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Philippines</v>
       </c>
       <c r="B135" t="str">
-        <f t="shared" si="4"/>
-        <v>return "PHIL";</v>
+        <f t="shared" si="5"/>
+        <v>PHIL</v>
       </c>
       <c r="C135" t="s">
         <v>125</v>
@@ -2732,12 +2742,12 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Poland</v>
       </c>
       <c r="B136" t="str">
-        <f t="shared" si="4"/>
-        <v>return "POLA";</v>
+        <f t="shared" si="5"/>
+        <v>POLA</v>
       </c>
       <c r="C136" t="s">
         <v>126</v>
@@ -2745,12 +2755,12 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Portugal</v>
       </c>
       <c r="B137" t="str">
-        <f t="shared" si="4"/>
-        <v>return "PORT";</v>
+        <f t="shared" si="5"/>
+        <v>PORT</v>
       </c>
       <c r="C137" t="s">
         <v>127</v>
@@ -2758,12 +2768,12 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Qatar</v>
       </c>
       <c r="B138" t="str">
-        <f t="shared" si="4"/>
-        <v>return "QATA";</v>
+        <f t="shared" si="5"/>
+        <v>QATA</v>
       </c>
       <c r="C138" t="s">
         <v>128</v>
@@ -2771,12 +2781,12 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Republic_of_the_Congo</v>
       </c>
       <c r="B139" t="str">
-        <f t="shared" si="4"/>
-        <v>return "REPU";</v>
+        <f t="shared" si="5"/>
+        <v>REPU</v>
       </c>
       <c r="C139" t="s">
         <v>129</v>
@@ -2784,12 +2794,12 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Romania</v>
       </c>
       <c r="B140" t="str">
-        <f t="shared" si="4"/>
-        <v>return "ROMA";</v>
+        <f t="shared" si="5"/>
+        <v>ROMA</v>
       </c>
       <c r="C140" t="s">
         <v>130</v>
@@ -2797,12 +2807,12 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Russia</v>
       </c>
       <c r="B141" t="str">
-        <f t="shared" si="4"/>
-        <v>return "RUSS";</v>
+        <f t="shared" si="5"/>
+        <v>RUSS</v>
       </c>
       <c r="C141" t="s">
         <v>131</v>
@@ -2810,12 +2820,12 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Rwanda</v>
       </c>
       <c r="B142" t="str">
-        <f t="shared" si="4"/>
-        <v>return "RWAN";</v>
+        <f t="shared" si="5"/>
+        <v>RWAN</v>
       </c>
       <c r="C142" t="s">
         <v>132</v>
@@ -2823,12 +2833,12 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Saint_Kitts_and_Nevis</v>
       </c>
       <c r="B143" t="str">
-        <f t="shared" si="4"/>
-        <v>return "SAIN";</v>
+        <f t="shared" si="5"/>
+        <v>SAIN</v>
       </c>
       <c r="C143" t="s">
         <v>133</v>
@@ -2836,12 +2846,12 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Samoa</v>
       </c>
       <c r="B144" t="str">
-        <f t="shared" si="4"/>
-        <v>return "SAMO";</v>
+        <f t="shared" si="5"/>
+        <v>SAMO</v>
       </c>
       <c r="C144" t="s">
         <v>134</v>
@@ -2849,12 +2859,12 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>San_Marino</v>
       </c>
       <c r="B145" t="str">
-        <f t="shared" si="4"/>
-        <v>return "SAN_";</v>
+        <f t="shared" si="5"/>
+        <v>SAN_</v>
       </c>
       <c r="C145" t="s">
         <v>135</v>
@@ -2862,12 +2872,12 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Sao_Tome_and_Principe</v>
       </c>
       <c r="B146" t="str">
-        <f t="shared" si="4"/>
-        <v>return "SAO_";</v>
+        <f t="shared" si="5"/>
+        <v>SAO_</v>
       </c>
       <c r="C146" t="s">
         <v>136</v>
@@ -2875,12 +2885,12 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Saudi_Arabia</v>
       </c>
       <c r="B147" t="str">
-        <f t="shared" si="4"/>
-        <v>return "SAUD";</v>
+        <f t="shared" si="5"/>
+        <v>SAUD</v>
       </c>
       <c r="C147" t="s">
         <v>137</v>
@@ -2888,12 +2898,12 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Senegal</v>
       </c>
       <c r="B148" t="str">
-        <f t="shared" si="4"/>
-        <v>return "SENE";</v>
+        <f t="shared" si="5"/>
+        <v>SENE</v>
       </c>
       <c r="C148" t="s">
         <v>138</v>
@@ -2901,12 +2911,12 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Serbia</v>
       </c>
       <c r="B149" t="str">
-        <f t="shared" si="4"/>
-        <v>return "SERB";</v>
+        <f t="shared" si="5"/>
+        <v>SERB</v>
       </c>
       <c r="C149" t="s">
         <v>139</v>
@@ -2914,12 +2924,12 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Seychelles</v>
       </c>
       <c r="B150" t="str">
-        <f t="shared" si="4"/>
-        <v>return "SEYC";</v>
+        <f t="shared" si="5"/>
+        <v>SEYC</v>
       </c>
       <c r="C150" t="s">
         <v>140</v>
@@ -2927,12 +2937,12 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Sierra_Leone</v>
       </c>
       <c r="B151" t="str">
-        <f t="shared" si="4"/>
-        <v>return "SIER";</v>
+        <f t="shared" si="5"/>
+        <v>SIER</v>
       </c>
       <c r="C151" t="s">
         <v>141</v>
@@ -2940,12 +2950,12 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Singapore</v>
       </c>
       <c r="B152" t="str">
-        <f t="shared" si="4"/>
-        <v>return "SING";</v>
+        <f t="shared" si="5"/>
+        <v>SING</v>
       </c>
       <c r="C152" t="s">
         <v>142</v>
@@ -2953,12 +2963,11 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Slovakia</v>
       </c>
-      <c r="B153" t="str">
-        <f t="shared" si="4"/>
-        <v>return "SLOV";</v>
+      <c r="B153" t="s">
+        <v>193</v>
       </c>
       <c r="C153" t="s">
         <v>143</v>
@@ -2966,12 +2975,12 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Slovenia</v>
       </c>
       <c r="B154" t="str">
-        <f t="shared" si="4"/>
-        <v>return "SLOV";</v>
+        <f t="shared" si="5"/>
+        <v>SLOV</v>
       </c>
       <c r="C154" t="s">
         <v>144</v>
@@ -2979,25 +2988,25 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Solomon_Islands</v>
       </c>
       <c r="B155" t="str">
-        <f t="shared" si="4"/>
-        <v>return "SOLO";</v>
+        <f t="shared" si="5"/>
+        <v>SOLO</v>
       </c>
       <c r="C155" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Somalia</v>
       </c>
       <c r="B156" t="str">
-        <f t="shared" si="4"/>
-        <v>return "SOMA";</v>
+        <f t="shared" si="5"/>
+        <v>SOMA</v>
       </c>
       <c r="C156" t="s">
         <v>145</v>
@@ -3005,12 +3014,11 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>South_Africa</v>
       </c>
-      <c r="B157" t="str">
-        <f t="shared" si="4"/>
-        <v>return "SOUT";</v>
+      <c r="B157" t="s">
+        <v>194</v>
       </c>
       <c r="C157" t="s">
         <v>146</v>
@@ -3021,21 +3029,22 @@
         <f>SUBSTITUTE(C158, " ", "_")</f>
         <v>South_Korea</v>
       </c>
-      <c r="B158" t="s">
-        <v>187</v>
+      <c r="B158" t="str">
+        <f t="shared" si="5"/>
+        <v>SOUT</v>
       </c>
       <c r="C158" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Spain</v>
       </c>
       <c r="B159" t="str">
-        <f t="shared" si="4"/>
-        <v>return "SPAI";</v>
+        <f t="shared" si="5"/>
+        <v>SPAI</v>
       </c>
       <c r="C159" t="s">
         <v>147</v>
@@ -3043,12 +3052,12 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Sri_Lanka</v>
       </c>
       <c r="B160" t="str">
-        <f t="shared" si="4"/>
-        <v>return "SRI_";</v>
+        <f t="shared" si="5"/>
+        <v>SRI_</v>
       </c>
       <c r="C160" t="s">
         <v>148</v>
@@ -3056,12 +3065,12 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Sudan</v>
       </c>
       <c r="B161" t="str">
-        <f t="shared" si="4"/>
-        <v>return "SUDA";</v>
+        <f t="shared" si="5"/>
+        <v>SUDA</v>
       </c>
       <c r="C161" t="s">
         <v>149</v>
@@ -3069,12 +3078,12 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Suriname</v>
       </c>
       <c r="B162" t="str">
-        <f t="shared" si="4"/>
-        <v>return "SURI";</v>
+        <f t="shared" si="5"/>
+        <v>SURI</v>
       </c>
       <c r="C162" t="s">
         <v>150</v>
@@ -3082,12 +3091,12 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Sweden</v>
       </c>
       <c r="B163" t="str">
-        <f t="shared" si="4"/>
-        <v>return "SWED";</v>
+        <f t="shared" si="5"/>
+        <v>SWED</v>
       </c>
       <c r="C163" t="s">
         <v>151</v>
@@ -3095,12 +3104,12 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Switzerland</v>
       </c>
       <c r="B164" t="str">
-        <f t="shared" si="4"/>
-        <v>return "SWIT";</v>
+        <f t="shared" si="5"/>
+        <v>SWIT</v>
       </c>
       <c r="C164" t="s">
         <v>152</v>
@@ -3108,12 +3117,12 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Syria</v>
       </c>
       <c r="B165" t="str">
-        <f t="shared" si="4"/>
-        <v>return "SYRI";</v>
+        <f t="shared" si="5"/>
+        <v>SYRI</v>
       </c>
       <c r="C165" t="s">
         <v>153</v>
@@ -3121,12 +3130,12 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Tajikistan</v>
       </c>
       <c r="B166" t="str">
-        <f t="shared" si="4"/>
-        <v>return "TAJI";</v>
+        <f t="shared" si="5"/>
+        <v>TAJI</v>
       </c>
       <c r="C166" t="s">
         <v>154</v>
@@ -3134,12 +3143,12 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Tanzania</v>
       </c>
       <c r="B167" t="str">
-        <f t="shared" si="4"/>
-        <v>return "TANZ";</v>
+        <f t="shared" si="5"/>
+        <v>TANZ</v>
       </c>
       <c r="C167" t="s">
         <v>155</v>
@@ -3147,12 +3156,12 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Thailand</v>
       </c>
       <c r="B168" t="str">
-        <f t="shared" si="4"/>
-        <v>return "THAI";</v>
+        <f t="shared" si="5"/>
+        <v>THAI</v>
       </c>
       <c r="C168" t="s">
         <v>156</v>
@@ -3160,12 +3169,12 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Timor-Leste</v>
       </c>
       <c r="B169" t="str">
-        <f t="shared" si="4"/>
-        <v>return "TIMO";</v>
+        <f>UPPER(LEFT(A169,4))</f>
+        <v>TIMO</v>
       </c>
       <c r="C169" t="s">
         <v>157</v>
@@ -3173,12 +3182,12 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Togo</v>
       </c>
       <c r="B170" t="str">
-        <f t="shared" si="4"/>
-        <v>return "TOGO";</v>
+        <f t="shared" ref="B170:B188" si="6">UPPER(LEFT(A170,4))</f>
+        <v>TOGO</v>
       </c>
       <c r="C170" t="s">
         <v>158</v>
@@ -3186,12 +3195,12 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Tonga</v>
       </c>
       <c r="B171" t="str">
-        <f t="shared" si="4"/>
-        <v>return "TONG";</v>
+        <f t="shared" si="6"/>
+        <v>TONG</v>
       </c>
       <c r="C171" t="s">
         <v>159</v>
@@ -3199,12 +3208,12 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Trinidad_and_Tobago</v>
       </c>
       <c r="B172" t="str">
-        <f t="shared" si="4"/>
-        <v>return "TRIN";</v>
+        <f t="shared" si="6"/>
+        <v>TRIN</v>
       </c>
       <c r="C172" t="s">
         <v>160</v>
@@ -3212,12 +3221,12 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Tunisia</v>
       </c>
       <c r="B173" t="str">
-        <f t="shared" si="4"/>
-        <v>return "TUNI";</v>
+        <f t="shared" si="6"/>
+        <v>TUNI</v>
       </c>
       <c r="C173" t="s">
         <v>161</v>
@@ -3225,12 +3234,12 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Turkey</v>
       </c>
       <c r="B174" t="str">
-        <f t="shared" si="4"/>
-        <v>return "TURK";</v>
+        <f t="shared" si="6"/>
+        <v>TURK</v>
       </c>
       <c r="C174" t="s">
         <v>162</v>
@@ -3238,11 +3247,11 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Turkmenistan</v>
       </c>
       <c r="B175" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="C175" t="s">
         <v>163</v>
@@ -3250,12 +3259,12 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Tuvalu</v>
       </c>
       <c r="B176" t="str">
-        <f t="shared" si="4"/>
-        <v>return "TUVA";</v>
+        <f t="shared" si="6"/>
+        <v>TUVA</v>
       </c>
       <c r="C176" t="s">
         <v>164</v>
@@ -3263,12 +3272,12 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Uganda</v>
       </c>
       <c r="B177" t="str">
-        <f t="shared" si="4"/>
-        <v>return "UGAN";</v>
+        <f t="shared" si="6"/>
+        <v>UGAN</v>
       </c>
       <c r="C177" t="s">
         <v>165</v>
@@ -3276,12 +3285,12 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Ukraine</v>
       </c>
       <c r="B178" t="str">
-        <f t="shared" si="4"/>
-        <v>return "UKRA";</v>
+        <f t="shared" si="6"/>
+        <v>UKRA</v>
       </c>
       <c r="C178" t="s">
         <v>166</v>
@@ -3289,37 +3298,36 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>United_Arab_Emirates</v>
       </c>
-      <c r="B179" t="str">
-        <f t="shared" si="4"/>
-        <v>return "UNIT";</v>
+      <c r="B179" t="s">
+        <v>191</v>
       </c>
       <c r="C179" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>United_Kingdom</v>
       </c>
       <c r="B180" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="C180" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Uruguay</v>
       </c>
       <c r="B181" t="str">
-        <f t="shared" si="4"/>
-        <v>return "URUG";</v>
+        <f t="shared" si="6"/>
+        <v>URUG</v>
       </c>
       <c r="C181" t="s">
         <v>167</v>
@@ -3327,12 +3335,12 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Uzbekistan</v>
       </c>
       <c r="B182" t="str">
-        <f t="shared" si="4"/>
-        <v>return "UZBE";</v>
+        <f t="shared" si="6"/>
+        <v>UZBE</v>
       </c>
       <c r="C182" t="s">
         <v>168</v>
@@ -3340,12 +3348,12 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Vanuatu</v>
       </c>
       <c r="B183" t="str">
-        <f t="shared" si="4"/>
-        <v>return "VANU";</v>
+        <f t="shared" si="6"/>
+        <v>VANU</v>
       </c>
       <c r="C183" t="s">
         <v>169</v>
@@ -3353,12 +3361,12 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Venezuela</v>
       </c>
       <c r="B184" t="str">
-        <f t="shared" si="4"/>
-        <v>return "VENE";</v>
+        <f t="shared" si="6"/>
+        <v>VENE</v>
       </c>
       <c r="C184" t="s">
         <v>170</v>
@@ -3366,12 +3374,12 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Vietnam</v>
       </c>
       <c r="B185" t="str">
-        <f t="shared" si="4"/>
-        <v>return "VIET";</v>
+        <f t="shared" si="6"/>
+        <v>VIET</v>
       </c>
       <c r="C185" t="s">
         <v>171</v>
@@ -3379,12 +3387,12 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Yemen</v>
       </c>
       <c r="B186" t="str">
-        <f t="shared" si="4"/>
-        <v>return "YEME";</v>
+        <f t="shared" si="6"/>
+        <v>YEME</v>
       </c>
       <c r="C186" t="s">
         <v>172</v>
@@ -3392,12 +3400,12 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Zambia</v>
       </c>
       <c r="B187" t="str">
-        <f t="shared" ref="B187:B188" si="6">CONCATENATE("return """, UPPER(LEFT(A187,4)), """;")</f>
-        <v>return "ZAMB";</v>
+        <f t="shared" si="6"/>
+        <v>ZAMB</v>
       </c>
       <c r="C187" t="s">
         <v>173</v>
@@ -3405,12 +3413,12 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Zimbabwe</v>
       </c>
       <c r="B188" t="str">
         <f t="shared" si="6"/>
-        <v>return "ZIMB";</v>
+        <v>ZIMB</v>
       </c>
       <c r="C188" t="s">
         <v>174</v>

</xml_diff>